<commit_message>
Add download instructional search results
</commit_message>
<xml_diff>
--- a/metridoc-grails-rid/grails-app/conf/spreadsheet/Transaction_List.xlsx
+++ b/metridoc-grails-rid/grails-app/conf/spreadsheet/Transaction_List.xlsx
@@ -1,85 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23416"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="75" windowWidth="18195" windowHeight="11820"/>
+    <workbookView xWindow="480" yWindow="80" windowWidth="18200" windowHeight="11820"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
-  <si>
-    <t>Consultation Mode</t>
-  </si>
-  <si>
-    <t>Staff Pennkey</t>
-  </si>
-  <si>
-    <t>Service Provided</t>
-  </si>
-  <si>
-    <t>User Goal</t>
-  </si>
-  <si>
-    <t>Prep Time (enter in minutes)</t>
-  </si>
-  <si>
-    <t>Date of Consultation (mm/dd/yyyy)</t>
-  </si>
-  <si>
-    <t>Course Name</t>
-  </si>
-  <si>
-    <t>Course Number</t>
-  </si>
-  <si>
-    <t>Faculty Sponsor</t>
-  </si>
-  <si>
-    <t>Course Sponsor</t>
-  </si>
-  <si>
-    <t>User Question</t>
-  </si>
-  <si>
-    <t>Notes</t>
-  </si>
-  <si>
-    <t>Library Unit</t>
-  </si>
-  <si>
-    <t>User Name</t>
-  </si>
-  <si>
-    <t>Rank</t>
-  </si>
-  <si>
-    <t>School</t>
-  </si>
-  <si>
-    <t>Department</t>
-  </si>
-  <si>
-    <t>Interact Occurrences</t>
-  </si>
-  <si>
-    <t>Event Length (min)</t>
-  </si>
-</sst>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -155,7 +102,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -483,93 +430,55 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
+      <selection pane="bottomLeft" activeCell="X1" sqref="X1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.5" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="22" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="13" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="17.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="7.140625" style="1" customWidth="1"/>
-    <col min="20" max="16384" width="9.140625" style="1"/>
+    <col min="15" max="15" width="17.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="7.1640625" style="1" customWidth="1"/>
+    <col min="20" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="11" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A1" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="I1" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="J1" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="K1" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="L1" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="M1" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="N1" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="O1" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="P1" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q1" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="R1" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="S1" s="8" t="s">
-        <v>11</v>
-      </c>
+    <row r="1" spans="1:19" s="11" customFormat="1" ht="16" thickBot="1">
+      <c r="A1" s="7"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
+      <c r="O1" s="8"/>
+      <c r="P1" s="8"/>
+      <c r="Q1" s="8"/>
+      <c r="R1" s="8"/>
+      <c r="S1" s="8"/>
     </row>
     <row r="2" spans="1:19">
       <c r="C2" s="6"/>
@@ -586,14 +495,14 @@
     <row r="5" spans="1:19">
       <c r="C5" s="6"/>
     </row>
-    <row r="6" spans="1:19" ht="15">
+    <row r="6" spans="1:19" ht="16">
       <c r="C6" s="6"/>
       <c r="K6" s="3"/>
     </row>
     <row r="7" spans="1:19">
       <c r="C7" s="6"/>
     </row>
-    <row r="8" spans="1:19" ht="15">
+    <row r="8" spans="1:19" ht="16">
       <c r="C8" s="6"/>
       <c r="K8" s="3"/>
     </row>
@@ -639,7 +548,7 @@
       <c r="A21" s="2"/>
       <c r="C21" s="6"/>
     </row>
-    <row r="22" spans="1:3" ht="15">
+    <row r="22" spans="1:3" ht="16">
       <c r="B22" s="3"/>
       <c r="C22" s="6"/>
     </row>
@@ -652,14 +561,14 @@
     <row r="25" spans="1:3">
       <c r="C25" s="6"/>
     </row>
-    <row r="26" spans="1:3" ht="15">
+    <row r="26" spans="1:3" ht="16">
       <c r="B26" s="3"/>
       <c r="C26" s="6"/>
     </row>
     <row r="27" spans="1:3">
       <c r="C27" s="6"/>
     </row>
-    <row r="28" spans="1:3" ht="15">
+    <row r="28" spans="1:3" ht="16">
       <c r="B28" s="3"/>
       <c r="C28" s="6"/>
     </row>
@@ -692,7 +601,12 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="landscape" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
+  <pageSetup orientation="landscape" horizontalDpi="200" verticalDpi="200"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -702,9 +616,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -714,8 +633,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>